<commit_message>
dox_project: 1.chapter 5 dynamic table and images  finished chapter 8 100% prepare annotation and class
</commit_message>
<xml_diff>
--- a/files/foundation_select.xlsx
+++ b/files/foundation_select.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5214CC5-AE4F-45AA-B08B-45AF36F8C61A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214DB6E7-1EFD-4621-8114-B68E95A9E772}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2052" windowWidth="12204" windowHeight="7848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="foundation_select" sheetId="2" r:id="rId1"/>
@@ -238,74 +238,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -324,6 +256,7 @@
       <sheetName val="成果输出"/>
       <sheetName val="风机基础条件输入"/>
       <sheetName val="基础数据"/>
+      <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -335,6 +268,7 @@
         </row>
       </sheetData>
       <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -348,7 +282,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CCE8CF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -605,34 +539,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57EF433E-2707-4A7D-9AED-7CD432278350}">
   <dimension ref="A1:AA59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.21875" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.25" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -709,7 +643,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -780,7 +714,7 @@
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
     </row>
-    <row r="3" spans="1:27" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -851,7 +785,7 @@
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
     </row>
-    <row r="4" spans="1:27" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -922,7 +856,7 @@
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
     </row>
-    <row r="5" spans="1:27" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -993,7 +927,7 @@
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
     </row>
-    <row r="6" spans="1:27" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1064,7 +998,7 @@
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
     </row>
-    <row r="7" spans="1:27" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1135,7 +1069,7 @@
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
     </row>
-    <row r="8" spans="1:27" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1206,7 +1140,7 @@
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
     </row>
-    <row r="9" spans="1:27" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1277,7 +1211,7 @@
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
     </row>
-    <row r="10" spans="1:27" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1357,7 +1291,7 @@
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
     </row>
-    <row r="11" spans="1:27" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1437,7 +1371,7 @@
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
     </row>
-    <row r="12" spans="1:27" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1517,7 +1451,7 @@
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
     </row>
-    <row r="13" spans="1:27" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1597,7 +1531,7 @@
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
     </row>
-    <row r="14" spans="1:27" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1677,7 +1611,7 @@
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
     </row>
-    <row r="15" spans="1:27" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1757,7 +1691,7 @@
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
     </row>
-    <row r="16" spans="1:27" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1837,7 +1771,7 @@
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
     </row>
-    <row r="17" spans="1:27" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1917,7 +1851,7 @@
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1944,7 +1878,7 @@
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1971,7 +1905,7 @@
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1998,7 +1932,7 @@
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -2025,7 +1959,7 @@
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -2052,7 +1986,7 @@
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -2079,7 +2013,7 @@
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -2106,7 +2040,7 @@
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -2133,7 +2067,7 @@
       <c r="Z25" s="2"/>
       <c r="AA25" s="2"/>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -2160,7 +2094,7 @@
       <c r="Z26" s="2"/>
       <c r="AA26" s="2"/>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -2187,7 +2121,7 @@
       <c r="Z27" s="2"/>
       <c r="AA27" s="2"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -2214,7 +2148,7 @@
       <c r="Z28" s="2"/>
       <c r="AA28" s="2"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -2241,7 +2175,7 @@
       <c r="Z29" s="2"/>
       <c r="AA29" s="2"/>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -2268,7 +2202,7 @@
       <c r="Z30" s="2"/>
       <c r="AA30" s="2"/>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -2295,7 +2229,7 @@
       <c r="Z31" s="2"/>
       <c r="AA31" s="2"/>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -2322,7 +2256,7 @@
       <c r="Z32" s="2"/>
       <c r="AA32" s="2"/>
     </row>
-    <row r="33" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -2349,7 +2283,7 @@
       <c r="Z33" s="2"/>
       <c r="AA33" s="2"/>
     </row>
-    <row r="34" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -2376,7 +2310,7 @@
       <c r="Z34" s="2"/>
       <c r="AA34" s="2"/>
     </row>
-    <row r="35" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -2403,7 +2337,7 @@
       <c r="Z35" s="2"/>
       <c r="AA35" s="2"/>
     </row>
-    <row r="36" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -2430,7 +2364,7 @@
       <c r="Z36" s="2"/>
       <c r="AA36" s="2"/>
     </row>
-    <row r="37" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -2457,7 +2391,7 @@
       <c r="Z37" s="2"/>
       <c r="AA37" s="2"/>
     </row>
-    <row r="38" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -2484,7 +2418,7 @@
       <c r="Z38" s="2"/>
       <c r="AA38" s="2"/>
     </row>
-    <row r="39" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -2511,7 +2445,7 @@
       <c r="Z39" s="2"/>
       <c r="AA39" s="2"/>
     </row>
-    <row r="40" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -2538,7 +2472,7 @@
       <c r="Z40" s="2"/>
       <c r="AA40" s="2"/>
     </row>
-    <row r="41" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -2565,7 +2499,7 @@
       <c r="Z41" s="2"/>
       <c r="AA41" s="2"/>
     </row>
-    <row r="42" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -2592,7 +2526,7 @@
       <c r="Z42" s="2"/>
       <c r="AA42" s="2"/>
     </row>
-    <row r="43" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -2619,7 +2553,7 @@
       <c r="Z43" s="2"/>
       <c r="AA43" s="2"/>
     </row>
-    <row r="44" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -2646,7 +2580,7 @@
       <c r="Z44" s="2"/>
       <c r="AA44" s="2"/>
     </row>
-    <row r="45" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -2673,7 +2607,7 @@
       <c r="Z45" s="2"/>
       <c r="AA45" s="2"/>
     </row>
-    <row r="46" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -2700,7 +2634,7 @@
       <c r="Z46" s="2"/>
       <c r="AA46" s="2"/>
     </row>
-    <row r="47" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -2727,7 +2661,7 @@
       <c r="Z47" s="2"/>
       <c r="AA47" s="2"/>
     </row>
-    <row r="48" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -2754,7 +2688,7 @@
       <c r="Z48" s="2"/>
       <c r="AA48" s="2"/>
     </row>
-    <row r="49" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -2781,7 +2715,7 @@
       <c r="Z49" s="2"/>
       <c r="AA49" s="2"/>
     </row>
-    <row r="50" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -2808,7 +2742,7 @@
       <c r="Z50" s="2"/>
       <c r="AA50" s="2"/>
     </row>
-    <row r="51" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -2835,7 +2769,7 @@
       <c r="Z51" s="2"/>
       <c r="AA51" s="2"/>
     </row>
-    <row r="52" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -2862,7 +2796,7 @@
       <c r="Z52" s="2"/>
       <c r="AA52" s="2"/>
     </row>
-    <row r="53" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -2889,7 +2823,7 @@
       <c r="Z53" s="2"/>
       <c r="AA53" s="2"/>
     </row>
-    <row r="54" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -2916,7 +2850,7 @@
       <c r="Z54" s="2"/>
       <c r="AA54" s="2"/>
     </row>
-    <row r="55" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -2943,7 +2877,7 @@
       <c r="Z55" s="2"/>
       <c r="AA55" s="2"/>
     </row>
-    <row r="56" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -2970,7 +2904,7 @@
       <c r="Z56" s="2"/>
       <c r="AA56" s="2"/>
     </row>
-    <row r="57" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -2997,7 +2931,7 @@
       <c r="Z57" s="2"/>
       <c r="AA57" s="2"/>
     </row>
-    <row r="58" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -3024,7 +2958,7 @@
       <c r="Z58" s="2"/>
       <c r="AA58" s="2"/>
     </row>
-    <row r="59" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:27" x14ac:dyDescent="0.2">
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>

</xml_diff>